<commit_message>
15 Commit passed all test cases on local lets try jenkins :)
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/EmployeesExcel.xlsx
+++ b/src/test/resources/testdata/EmployeesExcel.xlsx
@@ -49,7 +49,7 @@
     <t>C:\Users\herra\OneDrive\Desktop\Cat.jpg</t>
   </si>
   <si>
-    <t>opipyt</t>
+    <t>opipyt12</t>
   </si>
   <si>
     <t>Syntax1234@</t>
@@ -61,7 +61,7 @@
     <t>dfsd</t>
   </si>
   <si>
-    <t>jgjgurf</t>
+    <t>jgjgurf12</t>
   </si>
   <si>
     <t>serr</t>
@@ -70,7 +70,7 @@
     <t>kkkj</t>
   </si>
   <si>
-    <t>hjhjkyu</t>
+    <t>hjhjkyu12</t>
   </si>
   <si>
     <t>test1212</t>
@@ -79,7 +79,7 @@
     <t>opoip</t>
   </si>
   <si>
-    <t>mvmmvmn</t>
+    <t>mvmmvmn12</t>
   </si>
 </sst>
 </file>
@@ -87,9 +87,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
@@ -108,6 +108,43 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -117,12 +154,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -130,8 +175,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -139,22 +185,39 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -168,22 +231,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -191,32 +238,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -224,29 +247,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -267,25 +267,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -297,109 +411,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -412,30 +436,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -461,20 +461,43 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -494,32 +517,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -541,11 +543,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -563,145 +563,145 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">

</xml_diff>

<commit_message>
17 Commit passed all test cases on local jenkins failed. couldn't find the Pic ile not found.no changes 2nd try
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/EmployeesExcel.xlsx
+++ b/src/test/resources/testdata/EmployeesExcel.xlsx
@@ -49,7 +49,7 @@
     <t>C:\Users\herra\OneDrive\Desktop\Cat.jpg</t>
   </si>
   <si>
-    <t>opipyt12</t>
+    <t>opipyt123</t>
   </si>
   <si>
     <t>Syntax1234@</t>
@@ -61,7 +61,7 @@
     <t>dfsd</t>
   </si>
   <si>
-    <t>jgjgurf12</t>
+    <t>jgjgurf123</t>
   </si>
   <si>
     <t>serr</t>
@@ -70,7 +70,7 @@
     <t>kkkj</t>
   </si>
   <si>
-    <t>hjhjkyu12</t>
+    <t>hjhjkyu123</t>
   </si>
   <si>
     <t>test1212</t>
@@ -79,7 +79,7 @@
     <t>opoip</t>
   </si>
   <si>
-    <t>mvmmvmn12</t>
+    <t>mvmmvmn123</t>
   </si>
 </sst>
 </file>
@@ -87,9 +87,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
@@ -108,92 +108,75 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -208,6 +191,37 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -215,29 +229,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -245,8 +244,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -267,19 +267,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -291,19 +387,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -315,31 +429,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -351,103 +441,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -461,27 +461,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -517,15 +500,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -537,6 +511,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -558,20 +547,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -581,130 +581,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>

</xml_diff>

<commit_message>
17 Commit passed all test cases on local jenkins failed. couldn't find the Pic ile not found. Changed pict location
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/EmployeesExcel.xlsx
+++ b/src/test/resources/testdata/EmployeesExcel.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>firstName</t>
   </si>
@@ -46,10 +46,10 @@
     <t>gfhk</t>
   </si>
   <si>
-    <t>C:\Users\herra\OneDrive\Desktop\Cat.jpg</t>
-  </si>
-  <si>
-    <t>opipyt123</t>
+    <t>"C:\Users\herra\OneDrive\Desktop\CucumberProjectHassan\pict\Cat.jpg"</t>
+  </si>
+  <si>
+    <t>opipyt1234</t>
   </si>
   <si>
     <t>Syntax1234@</t>
@@ -62,24 +62,6 @@
   </si>
   <si>
     <t>jgjgurf123</t>
-  </si>
-  <si>
-    <t>serr</t>
-  </si>
-  <si>
-    <t>kkkj</t>
-  </si>
-  <si>
-    <t>hjhjkyu123</t>
-  </si>
-  <si>
-    <t>test1212</t>
-  </si>
-  <si>
-    <t>opoip</t>
-  </si>
-  <si>
-    <t>mvmmvmn123</t>
   </si>
 </sst>
 </file>
@@ -87,10 +69,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -108,6 +90,50 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -116,24 +142,42 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -145,18 +189,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -169,7 +206,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -177,76 +229,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -267,97 +249,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -369,85 +429,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -458,15 +440,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -515,6 +488,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -526,15 +517,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -563,7 +545,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -581,130 +563,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1035,15 +1017,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="6"/>
   <cols>
-    <col min="4" max="4" width="48" customWidth="1"/>
+    <col min="4" max="4" width="65.8571428571429" customWidth="1"/>
     <col min="5" max="5" width="25.4285714285714" customWidth="1"/>
     <col min="6" max="6" width="20.1428571428571" customWidth="1"/>
     <col min="7" max="7" width="17.7142857142857" customWidth="1"/>
@@ -1118,52 +1100,6 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
119 Commit passed all test cases on local jenkins failed. couldn't find the Pic ile not found. Changed pict location to testdata folder
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/EmployeesExcel.xlsx
+++ b/src/test/resources/testdata/EmployeesExcel.xlsx
@@ -46,10 +46,10 @@
     <t>gfhk</t>
   </si>
   <si>
-    <t>"C:\Users\herra\OneDrive\Desktop\CucumberProjectHassan\pict\Cat.jpg"</t>
-  </si>
-  <si>
-    <t>opipyt1234</t>
+    <t>C:\Users\herra\OneDrive\Desktop\CucumberProjectHassan\src\test\resources\testdata\Cat.jpg</t>
+  </si>
+  <si>
+    <t>opipyt1291</t>
   </si>
   <si>
     <t>Syntax1234@</t>
@@ -61,7 +61,7 @@
     <t>dfsd</t>
   </si>
   <si>
-    <t>jgjgurf123</t>
+    <t>jgjgurf1291</t>
   </si>
 </sst>
 </file>
@@ -70,8 +70,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
@@ -90,6 +90,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -97,31 +120,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -129,22 +130,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -167,6 +152,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -181,24 +180,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -206,13 +213,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -228,7 +228,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -249,67 +249,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -321,115 +429,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -443,17 +443,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -491,8 +485,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -502,6 +496,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -523,15 +532,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -545,7 +545,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -563,130 +563,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1020,12 +1020,12 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="6"/>
   <cols>
-    <col min="4" max="4" width="65.8571428571429" customWidth="1"/>
+    <col min="4" max="4" width="93.8571428571429" customWidth="1"/>
     <col min="5" max="5" width="25.4285714285714" customWidth="1"/>
     <col min="6" max="6" width="20.1428571428571" customWidth="1"/>
     <col min="7" max="7" width="17.7142857142857" customWidth="1"/>

</xml_diff>

<commit_message>
119 Commit passed all test cases on local jenkins failed. couldn't find the Pic ile not found. picture was missing from GitHub/jenkins. manually selected the picture. commit and pushed it to GitHub.
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/EmployeesExcel.xlsx
+++ b/src/test/resources/testdata/EmployeesExcel.xlsx
@@ -49,7 +49,7 @@
     <t>C:\Users\herra\OneDrive\Desktop\CucumberProjectHassan\src\test\resources\testdata\Cat.jpg</t>
   </si>
   <si>
-    <t>opipyt1291</t>
+    <t>opipyt12913</t>
   </si>
   <si>
     <t>Syntax1234@</t>
@@ -61,7 +61,7 @@
     <t>dfsd</t>
   </si>
   <si>
-    <t>jgjgurf1291</t>
+    <t>jgjgurf12914</t>
   </si>
 </sst>
 </file>
@@ -70,9 +70,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -87,6 +87,98 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -99,35 +191,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -135,93 +212,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -249,187 +249,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -447,7 +447,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -467,6 +467,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -482,20 +491,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -515,21 +521,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -540,12 +531,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -563,130 +563,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1020,7 +1020,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="6"/>

</xml_diff>

<commit_message>
119 Commit passed all test cases on local jenkins failed. couldn't find the Pic ile not found. picture was missing from GitHub/jenkins.changed the pict link/path
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/EmployeesExcel.xlsx
+++ b/src/test/resources/testdata/EmployeesExcel.xlsx
@@ -46,10 +46,10 @@
     <t>gfhk</t>
   </si>
   <si>
-    <t>C:\Users\herra\OneDrive\Desktop\CucumberProjectHassan\src\test\resources\testdata\Cat.jpg</t>
-  </si>
-  <si>
-    <t>opipyt12913</t>
+    <t>src/test/resources/testdata/Cat.jpg</t>
+  </si>
+  <si>
+    <t>opipyt1291342</t>
   </si>
   <si>
     <t>Syntax1234@</t>
@@ -61,7 +61,7 @@
     <t>dfsd</t>
   </si>
   <si>
-    <t>jgjgurf12914</t>
+    <t>jgjgurf1291442</t>
   </si>
 </sst>
 </file>
@@ -69,8 +69,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
@@ -91,38 +91,30 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -151,21 +143,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -191,6 +168,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -199,29 +198,30 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -249,19 +249,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -273,163 +417,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -440,15 +440,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -491,17 +482,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -521,13 +506,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -540,20 +529,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -563,130 +563,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1020,7 +1020,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="6"/>

</xml_diff>

<commit_message>
26 Commit fixing file not found issue. creating new directory for the pict
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/EmployeesExcel.xlsx
+++ b/src/test/resources/testdata/EmployeesExcel.xlsx
@@ -46,10 +46,10 @@
     <t>gfhk</t>
   </si>
   <si>
-    <t>https://github.com/herrafiisdet/HRProjectCucumberJenkins/blob/4da818041b33dbe9781687de443025b924c91188/src/test/resources/testdata/Cat.jpg</t>
-  </si>
-  <si>
-    <t>opi1ff4</t>
+    <t>C:\Users\herra\OneDrive\Desktop\CucumberProjectHassan\src\test\resources\Docs.assets\Cat.jpg</t>
+  </si>
+  <si>
+    <t>opi1ff4dp</t>
   </si>
   <si>
     <t>Syntax1234@</t>
@@ -61,7 +61,7 @@
     <t>dfsd</t>
   </si>
   <si>
-    <t>jgjguk14</t>
+    <t>jgjguk14dp</t>
   </si>
 </sst>
 </file>
@@ -69,10 +69,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -91,22 +91,76 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -121,83 +175,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -212,13 +189,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -228,7 +198,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -249,67 +249,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -321,7 +387,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -333,19 +399,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -357,79 +429,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -440,54 +440,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -502,6 +454,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -523,6 +484,54 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -531,29 +540,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -563,130 +563,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>

</xml_diff>

<commit_message>
28 Commit fixing file not found issue. creating new directory for the pict
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/EmployeesExcel.xlsx
+++ b/src/test/resources/testdata/EmployeesExcel.xlsx
@@ -46,7 +46,7 @@
     <t>gfhk</t>
   </si>
   <si>
-    <t>C:\Users\herra\OneDrive\Desktop\CucumberProjectHassan\src\test\resources\Docs.assets\Cat.jpg</t>
+    <t>Docs/assets/images/cat1.jpg</t>
   </si>
   <si>
     <t>opi1ff4dp</t>
@@ -69,8 +69,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
@@ -90,8 +90,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -99,52 +123,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -189,6 +167,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -197,38 +183,52 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -249,19 +249,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -273,163 +393,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -440,6 +440,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -454,15 +469,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -506,26 +512,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -540,20 +531,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -563,130 +563,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1020,7 +1020,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="6"/>

</xml_diff>

<commit_message>
31 removed the picture link from the Excel file. and commented // the step under addemployeesteps. will run without until we find a solution
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/EmployeesExcel.xlsx
+++ b/src/test/resources/testdata/EmployeesExcel.xlsx
@@ -65,7 +65,7 @@
     <t>jgjguk14dp3</t>
   </si>
   <si>
-    <t>xczvc124121</t>
+    <t>xczvc1241210</t>
   </si>
 </sst>
 </file>
@@ -73,10 +73,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -94,53 +94,91 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -154,44 +192,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -210,29 +210,29 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -253,19 +253,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -283,157 +379,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -444,6 +444,78 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -472,84 +544,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -567,130 +567,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1120,7 +1120,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="5"/>

</xml_diff>

<commit_message>
32 removed the picture link from the Excel file. and commented // the step under addemployeesteps. will run without until we find a solution
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/EmployeesExcel.xlsx
+++ b/src/test/resources/testdata/EmployeesExcel.xlsx
@@ -65,7 +65,7 @@
     <t>jgjguk14dp3</t>
   </si>
   <si>
-    <t>xczvc1241210</t>
+    <t>xcGzvc1241</t>
   </si>
 </sst>
 </file>
@@ -73,10 +73,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -95,6 +95,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -102,44 +133,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -153,32 +147,61 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -200,39 +223,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -253,19 +253,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -277,163 +421,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -449,17 +449,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -481,6 +474,30 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -491,6 +508,24 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -509,55 +544,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -567,130 +567,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1120,7 +1120,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="5"/>

</xml_diff>